<commit_message>
ISS update all regions 20210402
</commit_message>
<xml_diff>
--- a/data/sources/Rt_regions_avg14_from_ISS.xlsx
+++ b/data/sources/Rt_regions_avg14_from_ISS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F929"/>
+  <dimension ref="A1:F946"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20800,17 +20800,17 @@
     <row r="926">
       <c r="A926" t="inlineStr">
         <is>
-          <t>Campania</t>
+          <t>Abruzzo</t>
         </is>
       </c>
       <c r="B926" t="n">
-        <v>1.22</v>
+        <v>0.83</v>
       </c>
       <c r="C926" t="n">
-        <v>0.96</v>
+        <v>0.72</v>
       </c>
       <c r="D926" t="n">
-        <v>1.46</v>
+        <v>0.93</v>
       </c>
       <c r="E926" s="2" t="n">
         <v>44265</v>
@@ -20822,17 +20822,17 @@
     <row r="927">
       <c r="A927" t="inlineStr">
         <is>
-          <t>Lombardia</t>
+          <t>Basilicata</t>
         </is>
       </c>
       <c r="B927" t="n">
-        <v>0.92</v>
+        <v>1.07</v>
       </c>
       <c r="C927" t="n">
-        <v>0.72</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D927" t="n">
-        <v>1.13</v>
+        <v>1.52</v>
       </c>
       <c r="E927" s="2" t="n">
         <v>44265</v>
@@ -20844,17 +20844,17 @@
     <row r="928">
       <c r="A928" t="inlineStr">
         <is>
-          <t>Piemonte</t>
+          <t>Bolzano</t>
         </is>
       </c>
       <c r="B928" t="n">
-        <v>0.98</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C928" t="n">
-        <v>0.74</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D928" t="n">
-        <v>1.22</v>
+        <v>1.02</v>
       </c>
       <c r="E928" s="2" t="n">
         <v>44265</v>
@@ -20866,22 +20866,396 @@
     <row r="929">
       <c r="A929" t="inlineStr">
         <is>
-          <t>Toscana</t>
+          <t>Calabria</t>
         </is>
       </c>
       <c r="B929" t="n">
-        <v>1.06</v>
+        <v>1.29</v>
       </c>
       <c r="C929" t="n">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="D929" t="n">
-        <v>1.11</v>
+        <v>1.71</v>
       </c>
       <c r="E929" s="2" t="n">
         <v>44265</v>
       </c>
       <c r="F929" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>Campania</t>
+        </is>
+      </c>
+      <c r="B930" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="C930" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="D930" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="E930" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F930" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>Emilia R.</t>
+        </is>
+      </c>
+      <c r="B931" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="C931" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D931" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="E931" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F931" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>Friuli V.G.</t>
+        </is>
+      </c>
+      <c r="B932" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C932" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="D932" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="E932" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F932" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="B933" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="C933" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D933" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="E933" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F933" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>Liguria</t>
+        </is>
+      </c>
+      <c r="B934" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C934" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D934" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E934" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F934" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>Lombardia</t>
+        </is>
+      </c>
+      <c r="B935" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="C935" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="D935" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E935" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F935" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>Marche</t>
+        </is>
+      </c>
+      <c r="B936" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C936" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="D936" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="E936" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F936" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>Molise</t>
+        </is>
+      </c>
+      <c r="B937" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="C937" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D937" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="E937" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F937" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>Piemonte</t>
+        </is>
+      </c>
+      <c r="B938" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="C938" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="D938" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="E938" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F938" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>Puglia</t>
+        </is>
+      </c>
+      <c r="B939" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C939" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D939" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E939" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F939" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>Sardegna</t>
+        </is>
+      </c>
+      <c r="B940" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="C940" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="D940" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="E940" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F940" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>Sicilia</t>
+        </is>
+      </c>
+      <c r="B941" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="C941" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="D941" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="E941" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F941" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>Toscana</t>
+        </is>
+      </c>
+      <c r="B942" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="C942" t="n">
+        <v>1</v>
+      </c>
+      <c r="D942" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="E942" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F942" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>Trento</t>
+        </is>
+      </c>
+      <c r="B943" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="C943" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D943" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="E943" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F943" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>Umbria</t>
+        </is>
+      </c>
+      <c r="B944" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="C944" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D944" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="E944" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F944" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>Valle d'Aosta</t>
+        </is>
+      </c>
+      <c r="B945" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="C945" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="D945" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E945" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F945" s="2" t="n">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>Veneto</t>
+        </is>
+      </c>
+      <c r="B946" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="C946" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D946" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="E946" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="F946" s="2" t="n">
         <v>44278</v>
       </c>
     </row>

</xml_diff>